<commit_message>
view a specific plan
</commit_message>
<xml_diff>
--- a/api/mobile/modelling/mobile3.xlsx
+++ b/api/mobile/modelling/mobile3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="84">
   <si>
     <t>Who</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>produce json</t>
+  </si>
+  <si>
+    <t>4 + 4</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,6 +768,9 @@
       <c r="F4" s="1">
         <v>5</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E5" s="2"/>

</xml_diff>

<commit_message>
view plan of a number
</commit_message>
<xml_diff>
--- a/api/mobile/modelling/mobile3.xlsx
+++ b/api/mobile/modelling/mobile3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
   <si>
     <t>Who</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>other user wants to view summary of a number</t>
+  </si>
+  <si>
+    <t>refactor 10</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,23 +901,28 @@
       <c r="G11" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="H11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>201400404</v>
       </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -932,23 +940,31 @@
       <c r="E13" s="2">
         <v>200404</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="F13" s="1">
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>204400404</v>
       </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E15" s="2"/>

</xml_diff>

<commit_message>
view refill of a purchase
</commit_message>
<xml_diff>
--- a/api/mobile/modelling/mobile3.xlsx
+++ b/api/mobile/modelling/mobile3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
   <si>
     <t>Who</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>/numbers/{nid}/purchases/{pid}</t>
-  </si>
-  <si>
-    <t>view a puchase on a number</t>
   </si>
   <si>
     <t>/numbers/{nid}/purchases/{pid}/refill</t>
@@ -671,14 +668,14 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" style="1"/>
   </cols>
@@ -726,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -752,7 +749,7 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -775,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -801,10 +798,10 @@
         <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" t="s">
         <v>80</v>
-      </c>
-      <c r="H6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -850,7 +847,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -867,7 +864,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" s="2">
         <v>200</v>
@@ -890,7 +887,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E11" s="2">
         <v>404</v>
@@ -902,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1003,32 +1000,40 @@
         <v>8</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="E17" s="6">
         <v>200404</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="F17" s="10">
+        <v>10</v>
+      </c>
+      <c r="G17" s="10">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E18" s="6">
         <v>200404</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="F18" s="10">
+        <v>15</v>
+      </c>
+      <c r="G18" s="10">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -1047,7 +1052,7 @@
         <v>201400404</v>
       </c>
       <c r="F19" s="10">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G19" s="10">
         <v>16</v>
@@ -1213,13 +1218,13 @@
         <v>21</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="E30" s="6">
         <v>200404</v>

</xml_diff>

<commit_message>
topups post & get
</commit_message>
<xml_diff>
--- a/api/mobile/modelling/mobile3.xlsx
+++ b/api/mobile/modelling/mobile3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>Who</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>refactor 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 + </t>
   </si>
 </sst>
 </file>
@@ -667,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="112" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1154,6 +1157,12 @@
       <c r="E25" s="2">
         <v>201400404</v>
       </c>
+      <c r="F25" s="1">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
@@ -1171,8 +1180,12 @@
       <c r="E26" s="8">
         <v>200404</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1">
+        <v>5</v>
+      </c>
+      <c r="G26" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
@@ -1190,8 +1203,12 @@
       <c r="E27" s="8">
         <v>200404</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>

</xml_diff>